<commit_message>
Recreate baseline and match dac scenario pars
</commit_message>
<xml_diff>
--- a/tutorial/dac_scenarios/get_report_output.xlsx
+++ b/tutorial/dac_scenarios/get_report_output.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,48 +443,42 @@
         </is>
       </c>
       <c r="B1" s="1" t="n">
-        <v>2015</v>
+        <v>2025</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>2025</v>
+        <v>2035</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>2035</v>
+        <v>2045</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>2040</v>
+        <v>2050</v>
       </c>
       <c r="H1" s="1" t="n">
-        <v>2045</v>
+        <v>2055</v>
       </c>
       <c r="I1" s="1" t="n">
-        <v>2050</v>
+        <v>2060</v>
       </c>
       <c r="J1" s="1" t="n">
-        <v>2055</v>
+        <v>2070</v>
       </c>
       <c r="K1" s="1" t="n">
-        <v>2060</v>
+        <v>2080</v>
       </c>
       <c r="L1" s="1" t="n">
-        <v>2070</v>
+        <v>2090</v>
       </c>
       <c r="M1" s="1" t="n">
-        <v>2080</v>
+        <v>2100</v>
       </c>
       <c r="N1" s="1" t="n">
-        <v>2090</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>2100</v>
-      </c>
-      <c r="P1" s="1" t="n">
         <v>2110</v>
       </c>
     </row>
@@ -533,12 +527,6 @@
       <c r="N2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -577,19 +565,13 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>85.43864195936955</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>1080.843767980007</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>1767.08948025552</v>
-      </c>
-      <c r="O3" t="n">
-        <v>2208.752176092928</v>
-      </c>
-      <c r="P3" t="n">
-        <v>1346.567096455011</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -637,12 +619,6 @@
       <c r="N4" t="n">
         <v>0</v>
       </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -689,12 +665,6 @@
       <c r="N5" t="n">
         <v>0</v>
       </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -724,28 +694,22 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>10.38440193519746</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>36.64628950016741</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>66.35194562729849</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>433.6189440561302</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>947.4023463493324</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>720.9322472253007</v>
-      </c>
-      <c r="O6" t="n">
-        <v>572.1227030651112</v>
-      </c>
-      <c r="P6" t="n">
-        <v>342.5509961019926</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -785,19 +749,13 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>447.3610858414128</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>447.3610858414128</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>267.8516072710452</v>
-      </c>
-      <c r="O7" t="n">
-        <v>160.3726515075459</v>
-      </c>
-      <c r="P7" t="n">
-        <v>138.2871193323765</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -845,12 +803,6 @@
       <c r="N8" t="n">
         <v>0</v>
       </c>
-      <c r="O8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>1042.753026329113</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -897,12 +849,6 @@
       <c r="N9" t="n">
         <v>0</v>
       </c>
-      <c r="O9" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>304.1150318589819</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -949,12 +895,6 @@
       <c r="N10" t="n">
         <v>0</v>
       </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1001,12 +941,6 @@
       <c r="N11" t="n">
         <v>0</v>
       </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1053,12 +987,6 @@
       <c r="N12" t="n">
         <v>0</v>
       </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1088,28 +1016,22 @@
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>10.38440193519746</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>36.64628950016741</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>66.35194562729849</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>966.4186718569125</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>2475.607200170752</v>
+        <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>2755.873334751866</v>
-      </c>
-      <c r="O13" t="n">
-        <v>2941.247530665586</v>
-      </c>
-      <c r="P13" t="n">
-        <v>3174.273270077474</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1123,7 +1045,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1138,48 +1060,42 @@
         </is>
       </c>
       <c r="B1" s="1" t="n">
-        <v>2015</v>
+        <v>2025</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>2025</v>
+        <v>2035</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>2035</v>
+        <v>2045</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>2040</v>
+        <v>2050</v>
       </c>
       <c r="H1" s="1" t="n">
-        <v>2045</v>
+        <v>2055</v>
       </c>
       <c r="I1" s="1" t="n">
-        <v>2050</v>
+        <v>2060</v>
       </c>
       <c r="J1" s="1" t="n">
-        <v>2055</v>
+        <v>2070</v>
       </c>
       <c r="K1" s="1" t="n">
-        <v>2060</v>
+        <v>2080</v>
       </c>
       <c r="L1" s="1" t="n">
-        <v>2070</v>
+        <v>2090</v>
       </c>
       <c r="M1" s="1" t="n">
-        <v>2080</v>
+        <v>2100</v>
       </c>
       <c r="N1" s="1" t="n">
-        <v>2090</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>2100</v>
-      </c>
-      <c r="P1" s="1" t="n">
         <v>2110</v>
       </c>
     </row>
@@ -1228,12 +1144,6 @@
       <c r="N2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1272,18 +1182,12 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>8.543864195936955</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>99.5405126020637</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>72.8965033255198</v>
-      </c>
-      <c r="O3" t="n">
-        <v>98.20845798274119</v>
-      </c>
-      <c r="P3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1332,12 +1236,6 @@
       <c r="N4" t="n">
         <v>0</v>
       </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1384,12 +1282,6 @@
       <c r="N5" t="n">
         <v>0</v>
       </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1419,28 +1311,22 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>2.076880387039491</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>5.252377512993991</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>5.941131225426216</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>36.72669984288317</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>53.72987480108848</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>30.34733290596689</v>
-      </c>
-      <c r="P6" t="n">
-        <v>3.907766704232376</v>
       </c>
     </row>
     <row r="7">
@@ -1480,18 +1366,12 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>44.73610858414128</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>4.417106435033879</v>
-      </c>
-      <c r="O7" t="n">
-        <v>11.62015871572071</v>
-      </c>
-      <c r="P7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1540,12 +1420,6 @@
       <c r="N8" t="n">
         <v>0</v>
       </c>
-      <c r="O8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>104.2753026329113</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1592,12 +1466,6 @@
       <c r="N9" t="n">
         <v>0</v>
       </c>
-      <c r="O9" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>30.41150318589819</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1644,12 +1512,6 @@
       <c r="N10" t="n">
         <v>0</v>
       </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1696,12 +1558,6 @@
       <c r="N11" t="n">
         <v>0</v>
       </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1748,12 +1604,6 @@
       <c r="N12" t="n">
         <v>0</v>
       </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1783,28 +1633,22 @@
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>2.076880387039491</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>5.252377512993991</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>5.941131225426216</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>90.0066726229614</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>153.2703874031522</v>
+        <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>77.31360976055367</v>
-      </c>
-      <c r="O13" t="n">
-        <v>140.1759496044288</v>
-      </c>
-      <c r="P13" t="n">
-        <v>138.5945725230418</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1818,7 +1662,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1833,48 +1677,42 @@
         </is>
       </c>
       <c r="B1" s="1" t="n">
-        <v>2015</v>
+        <v>2025</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>2025</v>
+        <v>2035</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>2035</v>
+        <v>2045</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>2040</v>
+        <v>2050</v>
       </c>
       <c r="H1" s="1" t="n">
-        <v>2045</v>
+        <v>2055</v>
       </c>
       <c r="I1" s="1" t="n">
-        <v>2050</v>
+        <v>2060</v>
       </c>
       <c r="J1" s="1" t="n">
-        <v>2055</v>
+        <v>2070</v>
       </c>
       <c r="K1" s="1" t="n">
-        <v>2060</v>
+        <v>2080</v>
       </c>
       <c r="L1" s="1" t="n">
-        <v>2070</v>
+        <v>2090</v>
       </c>
       <c r="M1" s="1" t="n">
-        <v>2080</v>
+        <v>2100</v>
       </c>
       <c r="N1" s="1" t="n">
-        <v>2090</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>2100</v>
-      </c>
-      <c r="P1" s="1" t="n">
         <v>2110</v>
       </c>
     </row>
@@ -1923,12 +1761,6 @@
       <c r="N2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1967,18 +1799,12 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>16229.04440858966</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>170997.7599242198</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>113252.8823245675</v>
-      </c>
-      <c r="O3" t="n">
-        <v>137988.6777647724</v>
-      </c>
-      <c r="P3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2027,12 +1853,6 @@
       <c r="N4" t="n">
         <v>0</v>
       </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -2079,12 +1899,6 @@
       <c r="N5" t="n">
         <v>0</v>
       </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -2114,28 +1928,22 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>4823.322088295869</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>11600.23289911811</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>12478.31238217454</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>69762.25617145706</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>92300.99375442068</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>42639.79322552493</v>
-      </c>
-      <c r="P6" t="n">
-        <v>4965.638228735123</v>
       </c>
     </row>
     <row r="7">
@@ -2175,18 +1983,12 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>84976.10404725061</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>6862.469562745855</v>
-      </c>
-      <c r="O7" t="n">
-        <v>16327.00858495183</v>
-      </c>
-      <c r="P7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2235,12 +2037,6 @@
       <c r="N8" t="n">
         <v>0</v>
       </c>
-      <c r="O8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>132503.6698086667</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -2287,12 +2083,6 @@
       <c r="N9" t="n">
         <v>0</v>
       </c>
-      <c r="O9" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>38644.20121335269</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -2339,12 +2129,6 @@
       <c r="N10" t="n">
         <v>0</v>
       </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -2391,12 +2175,6 @@
       <c r="N11" t="n">
         <v>0</v>
       </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -2443,12 +2221,6 @@
       <c r="N12" t="n">
         <v>0</v>
       </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -2478,28 +2250,22 @@
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>4823.322088295869</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>11600.23289911811</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>12478.31238217454</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>170967.4046272973</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>263298.7536786405</v>
+        <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>120115.3518873133</v>
-      </c>
-      <c r="O13" t="n">
-        <v>196955.4795752491</v>
-      </c>
-      <c r="P13" t="n">
-        <v>176113.5092507545</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2644,19 +2410,19 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>78.00548010890439</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>986.8103601657459</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>1613.352695473289</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>2016.590736772843</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>1229.415759063425</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2773,28 +2539,28 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>9.480958966835276</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>33.45806231365285</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>60.57932635772352</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>395.8940959232468</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>864.9783422169405</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>658.2111417166994</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>522.3480278984466</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>312.7490594411192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2828,19 +2594,19 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>408.4406713732099</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>408.4406713732099</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>244.5485174384642</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>146.4202308263894</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>126.2561399504597</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2886,7 +2652,7 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>952.0335130384799</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2932,7 +2698,7 @@
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>277.6570240872504</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -3095,28 +2861,28 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>9.480958966835276</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>33.45806231365285</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>60.57932635772352</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>882.3402474053611</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>2260.229373755897</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>2516.112354628453</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>2685.35899549768</v>
+        <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>2898.111495580734</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set node_rel and node_loc equal
set node_rel and node_loc equal to fully reproduce results behaviour
</commit_message>
<xml_diff>
--- a/tutorial/dac_scenarios/get_report_output.xlsx
+++ b/tutorial/dac_scenarios/get_report_output.xlsx
@@ -489,43 +489,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.03192683931804503</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.6421116143994228</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1.266626409862353</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>2.444955656598223</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>4.668217337186446</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>8.863048717349876</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>16.77782117155247</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>31.71134705724933</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>102.3379908040818</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>329.9420322643048</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1063.427257397211</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>2545.467977962364</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>2032.82116599549</v>
       </c>
     </row>
     <row r="3">
@@ -544,34 +544,34 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.1951107636166253</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1.144474502355429</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>2.935725994351259</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>6.315444195764529</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>12.69226798181876</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>42.92921987589357</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>140.3719424438682</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>454.3944740377329</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>1466.375130467265</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>1375.164324299622</v>
       </c>
     </row>
     <row r="4">
@@ -584,40 +584,40 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.00832013724340157</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.09894068077803235</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.2699227577083377</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.5925302977991638</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1.201223482441415</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>2.34970064737567</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>4.516637671897544</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>14.77278896785996</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>47.82464250285461</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>154.3387714947697</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>237.1757854849172</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>420.6496069519287</v>
       </c>
     </row>
     <row r="5">
@@ -630,40 +630,40 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.1705807431751008</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.4643803156869322</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1.018718870168363</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>2.064640177532373</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>4.038075675305758</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>7.761537121642568</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>14.78693276188491</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>48.02499393272711</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>155.1392025577843</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>500.3294238044214</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>1373.86758678948</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>1477.091646810583</v>
       </c>
     </row>
     <row r="6">
@@ -676,40 +676,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.4927437130866399</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1.17978390228413</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>2.476085534360359</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>4.921936516216769</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>9.536747511915785</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>18.24393396113291</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>34.67257988663013</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>112.389976150087</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>362.8449396442537</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>1169.970393593092</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>2710.197870741217</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>2150.600259812235</v>
       </c>
     </row>
     <row r="7">
@@ -719,43 +719,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.02444303768772006</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.7922271641676304</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1.681085180002876</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>3.358174984541308</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>6.522493877299199</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>12.49290406521413</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>23.75782363243607</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>45.01237882411158</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>145.5449454584486</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>469.5249231332411</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>1513.594814593753</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>4123.44091719734</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>5594.135919941928</v>
       </c>
     </row>
     <row r="8">
@@ -765,43 +765,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.0252984265455309</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>2.096199403634548</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>4.759825782014541</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>9.785533558394343</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>19.2679965864584</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>37.15942781952787</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>70.91682931113232</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>134.6100096174165</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>435.8999765451067</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>1406.848197870359</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>4535.861945350807</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>9405.134321401261</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>9315.136706420724</v>
       </c>
     </row>
     <row r="9">
@@ -817,37 +817,37 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.04530537974837011</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.2929358916521486</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.760163052129754</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1.641723316289733</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>3.305043784542053</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>6.443382809774082</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>21.30624536700153</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>69.20385746108481</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>223.5604785683471</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>720.9958503537005</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>1346.581622336518</v>
       </c>
     </row>
     <row r="10">
@@ -884,16 +884,16 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>0.6438220879409279</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>2.718627025890233</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>2.396715981919769</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>1.435002391238348</v>
       </c>
     </row>
     <row r="11">
@@ -930,16 +930,16 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>0.4092284375570817</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>1.728023177433443</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>1.523408958654902</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>0.9121212171133624</v>
       </c>
     </row>
     <row r="12">
@@ -955,37 +955,37 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.007258226268384626</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.6141808028322584</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1.759317199383736</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>3.919950890308719</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>7.996616307999211</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>15.68843422123317</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>52.1257047758435</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>169.5498042097182</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>547.9650619385075</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>1767.460105735589</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>1745.940780484399</v>
       </c>
     </row>
     <row r="13">
@@ -995,43 +995,43 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>0.08166830355129599</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>4.202182775706744</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>9.50320587664562</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>20.45561881987197</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>41.70176954636128</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>81.78882747270453</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>157.4247501335778</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>300.1339708320161</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>975.3318418770497</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>3152.302592612967</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>10167.88927098196</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>24354.03567107371</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>25460.46915666178</v>
       </c>
     </row>
   </sheetData>
@@ -1106,43 +1106,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.006385367863609007</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.1220369550162755</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.124902959092586</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.2356658493471741</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.4446523361176445</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.845351643896295</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1.704991445856794</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>3.11160813623196</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>7.29166038338624</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>23.72049091346406</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>78.97640463456391</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>163.7101477049405</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>0.08376657732652526</v>
       </c>
     </row>
     <row r="3">
@@ -1161,34 +1161,34 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.03902215272332507</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.1898727477477608</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.358250298399166</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>0.6759436402826541</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1.275364757210847</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>3.090674452706084</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>10.13985150300465</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>33.7542586744156</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>107.8133286208086</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>12.82597447194583</v>
       </c>
     </row>
     <row r="4">
@@ -1201,40 +1201,40 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.001664027448680314</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.01812410870692616</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.03419641538606107</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.06452150801816522</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.1217386369284503</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>0.2313594604355313</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>0.451511513611301</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>1.058843714293814</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>3.440024914077114</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>11.46443037825295</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>10.53313571320021</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>25.79960979286619</v>
       </c>
     </row>
     <row r="5">
@@ -1247,40 +1247,40 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.03411614863502015</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.05875991450236628</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.1108677108962861</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.209184261472802</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.394687099554677</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.7788084379023822</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1.463839042550835</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>3.431536037900564</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>11.15576258712685</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>37.16141177436501</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>94.64746561101961</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>34.48099318285622</v>
       </c>
     </row>
     <row r="6">
@@ -1293,40 +1293,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.09854874261732799</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.1374080378394981</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.2592603264152458</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>0.4891701963712818</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>0.9229621991398033</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>1.839986032460754</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>3.423137222938942</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>8.023662338646133</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>26.08926650619458</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>86.89594168379152</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>171.0792121372329</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>0.5328430020948771</v>
       </c>
     </row>
     <row r="7">
@@ -1336,43 +1336,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.004888607537544012</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.1535568252959821</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>0.1777716031670491</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>0.3354179609076866</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>0.6328637785515783</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1.198970645120531</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>2.40654073874037</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>4.428682641502151</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>10.37918158852545</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>33.75733421936251</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>112.4125564457501</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>283.0528681643027</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>220.154445607015</v>
       </c>
     </row>
     <row r="8">
@@ -1382,43 +1382,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.00505968530910618</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.4141801954178035</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.5327252756759985</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1.005141555275961</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>1.896492605612812</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>3.583345931923001</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>7.165660493738692</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>13.27136133693284</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>31.1056906218102</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>101.1520333733247</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>336.881315850851</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>553.0560996026129</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>210.016913114034</v>
       </c>
     </row>
     <row r="9">
@@ -1434,37 +1434,37 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.009061075949674022</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.04952610238075569</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.09344543209552107</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>0.1763120528319958</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>0.3326640936504641</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>0.6367288809960798</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>1.534410664937003</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>4.984444617260823</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>16.60439790710539</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>53.00296481963424</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>73.3529984604649</v>
       </c>
     </row>
     <row r="10">
@@ -1501,16 +1501,16 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>0.06438220879409279</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>0.2074804937949305</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>0.03975999222636958</v>
       </c>
     </row>
     <row r="11">
@@ -1547,16 +1547,16 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>0.04092284375570817</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>0.1318794739876362</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>0.02527238471751815</v>
       </c>
     </row>
     <row r="12">
@@ -1572,37 +1572,37 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.001451645253676925</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.1213845153127748</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>0.2290272793102955</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.4321267381849967</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>0.8153330835380983</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1.53981522790047</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>3.761676132944995</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>12.21956340319206</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>40.69610472418618</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>129.9401241477767</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>24.3059015385701</v>
       </c>
     </row>
     <row r="13">
@@ -1612,43 +1612,43 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>0.0163336607102592</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>0.8241028944310896</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1.060204620187775</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>2.19048258864527</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>4.249230145297861</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>8.033745245978915</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>15.95128742660574</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>29.60204875987543</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>69.67733593515047</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>226.7640770895571</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>755.1861820410643</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>1566.835346521528</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>601.6184781241175</v>
       </c>
     </row>
   </sheetData>
@@ -1723,43 +1723,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>19.06517595244923</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>311.2552537690108</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>280.8592918747708</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>458.7824922166112</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>779.5022243543979</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1318.215992942565</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>2471.333951026047</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>4168.216911052246</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>11453.50744761984</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>40038.76543247253</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>131537.0925193689</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>265412.2091320863</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>97.1717426960891</v>
       </c>
     </row>
     <row r="3">
@@ -1778,34 +1778,34 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>73.32184452407334</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>325.4058138175898</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>554.8043246158685</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>979.4017781511488</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1720.747637724019</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>3850.733114115564</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>12208.17841258754</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>40120.64940299713</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>175590.1776582799</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>17936.72272210229</v>
       </c>
     </row>
     <row r="4">
@@ -1818,40 +1818,40 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>4.477748101928343</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>42.51807157992635</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>68.42600129504662</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>115.1360501980951</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>190.8800957719636</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>335.4480816854768</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>601.3410942880751</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>1305.15193911284</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>5819.971750632224</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>16654.64725778939</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>17021.65264388867</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>41264.06386169812</v>
       </c>
     </row>
     <row r="5">
@@ -1864,40 +1864,40 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>91.80348552346207</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>137.8472338276812</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>221.8429634721417</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>373.2809472277563</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>618.8496377467558</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1129.194354114664</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1949.599390430903</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>4229.779951036992</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>13501.26167107028</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>50373.4987488886</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>152192.6528157138</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>53332.95291666834</v>
       </c>
     </row>
     <row r="6">
@@ -1910,40 +1910,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>251.348568045495</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>308.9784620466522</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>504.7150404488798</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>857.5447044506393</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1439.239564472635</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>2667.004554470889</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>4585.531929732318</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>9937.546516283395</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>41268.56137399755</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>145472.4959728354</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>276055.7877367791</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>618.1138677201203</v>
       </c>
     </row>
     <row r="7">
@@ -1953,43 +1953,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>16.39140330123432</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>429.378666029131</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>430.01706404887</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>684.7993715279603</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>1144.224040259039</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1887.647393971313</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>3490.013510136059</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>5872.654616763927</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>12747.50324339518</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>57210.5797416068</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>188854.0061290132</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>455298.0935393163</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>354844.9354293869</v>
       </c>
     </row>
     <row r="8">
@@ -1999,43 +1999,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>17.86063854429172</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1131.262793150509</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1243.860246175889</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1948.436750655791</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>3303.121171195834</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>5535.982797146482</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>10370.50214956332</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>17910.76383309782</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>38963.29912978567</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>170316.7592330028</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>461501.979952524</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>688909.3768437783</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>311817.7787036936</v>
       </c>
     </row>
     <row r="9">
@@ -2051,37 +2051,37 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>23.68166565903003</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>106.4840916847676</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>174.8177143643008</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>280.6076845642347</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>482.7188863733789</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>834.4968714334622</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>1866.395756402773</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>6070.704632700475</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>20330.75688541798</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>64709.89632939233</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>83986.2491172939</v>
       </c>
     </row>
     <row r="10">
@@ -2118,16 +2118,16 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>108.4846656401343</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>345.7849161536932</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>64.64338576132072</v>
       </c>
     </row>
     <row r="11">
@@ -2164,16 +2164,16 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>68.95540095680582</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>219.7890125530545</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>41.08885396912972</v>
       </c>
     </row>
     <row r="12">
@@ -2189,37 +2189,37 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>3.723324911155946</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>257.6932567832552</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>424.8685058485293</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>685.893165184136</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>1182.934157582085</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>2024.025524466052</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>6411.776968604743</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>20780.71171910246</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>69170.37165583186</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>208342.0968548207</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>38945.08064702537</v>
       </c>
     </row>
     <row r="13">
@@ -2229,43 +2229,43 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>53.31721779797528</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>2219.526514619537</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>2471.485360123976</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>4324.501812608527</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>7497.901171716181</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>12512.12065641595</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>23108.55142310307</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>39667.37780898883</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>90765.694066357</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>367392.9340337696</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>1124581.072453373</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>2303531.943554055</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>902948.8012480151</v>
       </c>
     </row>
   </sheetData>
@@ -2340,43 +2340,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.02915693088405939</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.5864033008213906</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1.156736447362879</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>2.232836216071437</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>4.263212180078946</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>8.094108417671119</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>15.32221111557303</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>28.96013429885784</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>93.45935233249475</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>301.3169244422875</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>971.166445111608</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>2324.628290376588</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>1856.45768584063</v>
       </c>
     </row>
     <row r="3">
@@ -2395,34 +2395,34 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.1781833457686076</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1.045182193931899</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>2.681028305343615</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>5.767528945903679</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>11.59111231216325</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>39.20476700994847</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>128.1935547432587</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>414.9721224088885</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>1339.15537028974</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>1255.857830410614</v>
       </c>
     </row>
     <row r="4">
@@ -2435,40 +2435,40 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.007598298852421526</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.09035678609865967</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.2465048015601257</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.5411235596339394</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1.09700774652184</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>2.145845340069105</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>4.124783262006889</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>13.49113147749768</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>43.67547260534667</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>140.948649766913</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>216.5988908538056</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>384.1548921935422</v>
       </c>
     </row>
     <row r="5">
@@ -2481,40 +2481,40 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.1557815006165304</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.4240916124994815</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.9303368677336648</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1.885516143865181</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>3.687740342744984</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>7.08816175492472</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>13.50404818436978</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>43.85844194769599</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>141.6796370390724</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>456.9218482232159</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>1254.673595241534</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>1348.942143206012</v>
       </c>
     </row>
     <row r="6">
@@ -2527,40 +2527,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.4499942585266118</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1.077428221264046</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>2.261265328182977</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>4.494919192892025</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>8.709358458370579</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>16.66112690514422</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>31.66445651747043</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>102.6392476256503</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>331.36524168425</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>1068.466112870403</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>2475.066548622116</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>1964.01850211163</v>
       </c>
     </row>
     <row r="7">
@@ -2570,43 +2570,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.02232240884723293</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.7234951270937264</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1.535237607308562</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>3.066826469900738</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>5.956615413058629</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>11.40904480841473</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>21.69664258669961</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>41.10719527316126</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>132.9177584095422</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>428.7898841399463</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>1382.278369492012</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>3765.699467760128</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>5108.799926887605</v>
       </c>
     </row>
     <row r="8">
@@ -2616,43 +2616,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.02310358588632959</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1.914337354917396</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>4.346872860287252</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>8.936560327300771</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>17.59634391457388</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>33.93555052011678</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>64.76422768139936</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>122.9315156323438</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>398.082170360828</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>1284.792874767451</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>4142.339676119458</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>8589.163763836768</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>8506.974161114817</v>
       </c>
     </row>
     <row r="9">
@@ -2668,37 +2668,37 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.04137477602590878</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>0.2675213622394051</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>0.694212832995209</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1.499290699807975</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>3.018304826065802</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>5.88436786280738</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>19.4577583260288</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>63.19986982747471</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>204.1648206103627</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>658.4436989531511</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>1229.754906243396</v>
       </c>
     </row>
     <row r="10">
@@ -2735,16 +2735,16 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>0.5879653771150026</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>2.482764407205692</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>2.188781718648191</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>1.310504466884336</v>
       </c>
     </row>
     <row r="11">
@@ -2781,16 +2781,16 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>0.3737246005087504</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>1.578103358386706</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>1.391241058132331</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>0.8329874128889153</v>
       </c>
     </row>
     <row r="12">
@@ -2806,37 +2806,37 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.006628517140077284</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.5608957103490945</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1.606682373866426</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>3.579863826765953</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>7.302845943378275</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>14.3273371883408</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>47.60338335693471</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>154.8400038444915</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>500.4247140990935</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>1614.118818023369</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>1594.466466195798</v>
       </c>
     </row>
     <row r="13">
@@ -2846,43 +2846,43 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>0.07458292561762192</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>3.837609840828077</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>8.678726827986868</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>18.68093042910682</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>38.08380780489613</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>74.69299312575758</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>143.7668950991578</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>274.0949505315215</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>890.7140108466208</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>2878.815153071203</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>9285.743626467547</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>22241.12846673398</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>23251.57000608382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add feature to allow multiple relation_activity data input feature
</commit_message>
<xml_diff>
--- a/tutorial/dac_scenarios/get_report_output.xlsx
+++ b/tutorial/dac_scenarios/get_report_output.xlsx
@@ -489,43 +489,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.03192683931804503</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6421116143994228</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1.266626409862353</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>2.444955656598223</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>4.668217337186446</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8.863048717349876</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>16.77782117155247</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>31.71134705724933</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>102.3379908040818</v>
+        <v>18.66377935190396</v>
       </c>
       <c r="K2" t="n">
-        <v>329.9420322643048</v>
+        <v>244.1504077286026</v>
       </c>
       <c r="L2" t="n">
-        <v>1063.427257397211</v>
+        <v>894.9093555782582</v>
       </c>
       <c r="M2" t="n">
-        <v>2545.467977962364</v>
+        <v>3271.574975976034</v>
       </c>
       <c r="N2" t="n">
-        <v>2032.82116599549</v>
+        <v>5744.733880686536</v>
       </c>
     </row>
     <row r="3">
@@ -544,34 +544,34 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1951107636166253</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1.144474502355429</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>2.935725994351259</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>6.315444195764529</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>12.69226798181876</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>42.92921987589357</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>140.3719424438682</v>
+        <v>98.46560893642852</v>
       </c>
       <c r="L3" t="n">
-        <v>454.3944740377329</v>
+        <v>581.2031918205647</v>
       </c>
       <c r="M3" t="n">
-        <v>1466.375130467265</v>
+        <v>2087.202376268372</v>
       </c>
       <c r="N3" t="n">
-        <v>1375.164324299622</v>
+        <v>1833.498068690948</v>
       </c>
     </row>
     <row r="4">
@@ -584,40 +584,40 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.00832013724340157</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.09894068077803235</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2699227577083377</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5925302977991638</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1.201223482441415</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>2.34970064737567</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>4.516637671897544</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>14.77278896785996</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>47.82464250285461</v>
+        <v>19.91721806661441</v>
       </c>
       <c r="L4" t="n">
-        <v>154.3387714947697</v>
+        <v>32.16473581348519</v>
       </c>
       <c r="M4" t="n">
-        <v>237.1757854849172</v>
+        <v>181.335333163807</v>
       </c>
       <c r="N4" t="n">
-        <v>420.6496069519287</v>
+        <v>165.2529652570644</v>
       </c>
     </row>
     <row r="5">
@@ -630,40 +630,40 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1705807431751008</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4643803156869322</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1.018718870168363</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>2.064640177532373</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>4.038075675305758</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>7.761537121642568</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>14.78693276188491</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>48.02499393272711</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>155.1392025577843</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>500.3294238044214</v>
+        <v>379.5991085184106</v>
       </c>
       <c r="M5" t="n">
-        <v>1373.86758678948</v>
+        <v>1614.023271211976</v>
       </c>
       <c r="N5" t="n">
-        <v>1477.091646810583</v>
+        <v>1424.223716952771</v>
       </c>
     </row>
     <row r="6">
@@ -676,40 +676,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4927437130866399</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1.17978390228413</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>2.476085534360359</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>4.921936516216769</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>9.536747511915785</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>18.24393396113291</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>34.67257988663013</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>112.389976150087</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>362.8449396442537</v>
+        <v>98.80521955702118</v>
       </c>
       <c r="L6" t="n">
-        <v>1169.970393593092</v>
+        <v>693.3143410238371</v>
       </c>
       <c r="M6" t="n">
-        <v>2710.197870741217</v>
+        <v>2127.374128422341</v>
       </c>
       <c r="N6" t="n">
-        <v>2150.600259812235</v>
+        <v>2228.199757930155</v>
       </c>
     </row>
     <row r="7">
@@ -719,43 +719,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.02444303768772006</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7922271641676304</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.681085180002876</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>3.358174984541308</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>6.522493877299199</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>12.49290406521413</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>23.75782363243607</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>45.01237882411158</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>145.5449454584486</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>469.5249231332411</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1513.594814593753</v>
+        <v>364.0305599183185</v>
       </c>
       <c r="M7" t="n">
-        <v>4123.44091719734</v>
+        <v>3193.816919241436</v>
       </c>
       <c r="N7" t="n">
-        <v>5594.135919941928</v>
+        <v>3011.801639282276</v>
       </c>
     </row>
     <row r="8">
@@ -765,43 +765,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0252984265455309</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>2.096199403634548</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>4.759825782014541</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>9.785533558394343</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>19.2679965864584</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>37.15942781952787</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>70.91682931113232</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>134.6100096174165</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>435.8999765451067</v>
+        <v>59.7911736963669</v>
       </c>
       <c r="K8" t="n">
-        <v>1406.848197870359</v>
+        <v>288.9724025148556</v>
       </c>
       <c r="L8" t="n">
-        <v>4535.861945350807</v>
+        <v>1579.359255871965</v>
       </c>
       <c r="M8" t="n">
-        <v>9405.134321401261</v>
+        <v>4797.305416290115</v>
       </c>
       <c r="N8" t="n">
-        <v>9315.136706420724</v>
+        <v>4671.706133528686</v>
       </c>
     </row>
     <row r="9">
@@ -817,37 +817,37 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.04530537974837011</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2929358916521486</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.760163052129754</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>1.641723316289733</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>3.305043784542053</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>6.443382809774082</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>21.30624536700153</v>
+        <v>3.529803798301121</v>
       </c>
       <c r="K9" t="n">
-        <v>69.20385746108481</v>
+        <v>14.30449694748633</v>
       </c>
       <c r="L9" t="n">
-        <v>223.5604785683471</v>
+        <v>56.8254426051115</v>
       </c>
       <c r="M9" t="n">
-        <v>720.9958503537005</v>
+        <v>411.2416289606244</v>
       </c>
       <c r="N9" t="n">
-        <v>1346.581622336518</v>
+        <v>383.7113586076439</v>
       </c>
     </row>
     <row r="10">
@@ -881,19 +881,19 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>37.62510653763389</v>
       </c>
       <c r="K10" t="n">
-        <v>0.6438220879409279</v>
+        <v>118.4880163297111</v>
       </c>
       <c r="L10" t="n">
-        <v>2.718627025890233</v>
+        <v>215.981506663179</v>
       </c>
       <c r="M10" t="n">
-        <v>2.396715981919769</v>
+        <v>714.7924211982361</v>
       </c>
       <c r="N10" t="n">
-        <v>1.435002391238348</v>
+        <v>616.2079445010551</v>
       </c>
     </row>
     <row r="11">
@@ -924,22 +924,22 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>49.15860199659996</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>184.0425282574486</v>
       </c>
       <c r="K11" t="n">
-        <v>0.4092284375570817</v>
+        <v>379.6026023193152</v>
       </c>
       <c r="L11" t="n">
-        <v>1.728023177433443</v>
+        <v>496.2806949768392</v>
       </c>
       <c r="M11" t="n">
-        <v>1.523408958654902</v>
+        <v>1746.590509890193</v>
       </c>
       <c r="N11" t="n">
-        <v>0.9121212171133624</v>
+        <v>1532.171143966986</v>
       </c>
     </row>
     <row r="12">
@@ -955,37 +955,37 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.007258226268384626</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.6141808028322584</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>1.759317199383736</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>3.919950890308719</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>7.996616307999211</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>15.68843422123317</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>52.1257047758435</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>169.5498042097182</v>
+        <v>68.82967782317435</v>
       </c>
       <c r="L12" t="n">
-        <v>547.9650619385075</v>
+        <v>223.8712925744189</v>
       </c>
       <c r="M12" t="n">
-        <v>1767.460105735589</v>
+        <v>825.3909585301852</v>
       </c>
       <c r="N12" t="n">
-        <v>1745.940780484399</v>
+        <v>713.4553122429758</v>
       </c>
     </row>
     <row r="13">
@@ -995,43 +995,43 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.08166830355129599</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>4.202182775706744</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>9.50320587664562</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>20.45561881987197</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>41.70176954636128</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>81.78882747270453</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>157.4247501335778</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>300.1339708320161</v>
+        <v>49.15860199659996</v>
       </c>
       <c r="J13" t="n">
-        <v>975.3318418770497</v>
+        <v>303.6523916416545</v>
       </c>
       <c r="K13" t="n">
-        <v>3152.302592612967</v>
+        <v>1331.535650223209</v>
       </c>
       <c r="L13" t="n">
-        <v>10167.88927098196</v>
+        <v>5517.539485364388</v>
       </c>
       <c r="M13" t="n">
-        <v>24354.03567107371</v>
+        <v>20970.64793915332</v>
       </c>
       <c r="N13" t="n">
-        <v>25460.46915666178</v>
+        <v>22324.9619216471</v>
       </c>
     </row>
   </sheetData>
@@ -1106,43 +1106,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.006385367863609007</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1220369550162755</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.124902959092586</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2356658493471741</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4446523361176445</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.845351643896295</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1.704991445856794</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>3.11160813623196</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>7.29166038338624</v>
+        <v>1.866377935190396</v>
       </c>
       <c r="K2" t="n">
-        <v>23.72049091346406</v>
+        <v>22.54866283766987</v>
       </c>
       <c r="L2" t="n">
-        <v>78.97640463456391</v>
+        <v>66.00908375256077</v>
       </c>
       <c r="M2" t="n">
-        <v>163.7101477049405</v>
+        <v>249.8740824262077</v>
       </c>
       <c r="N2" t="n">
-        <v>0.08376657732652526</v>
+        <v>291.5947637661656</v>
       </c>
     </row>
     <row r="3">
@@ -1161,34 +1161,34 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03902215272332507</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1898727477477608</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.358250298399166</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6759436402826541</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>1.275364757210847</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>3.090674452706084</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>10.13985150300465</v>
+        <v>9.846560893642852</v>
       </c>
       <c r="L3" t="n">
-        <v>33.7542586744156</v>
+        <v>48.27375828841362</v>
       </c>
       <c r="M3" t="n">
-        <v>107.8133286208086</v>
+        <v>155.5231988916021</v>
       </c>
       <c r="N3" t="n">
-        <v>12.82597447194583</v>
+        <v>3.68972883328588</v>
       </c>
     </row>
     <row r="4">
@@ -1201,40 +1201,40 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.001664027448680314</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01812410870692616</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03419641538606107</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.06452150801816522</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1217386369284503</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2313594604355313</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.451511513611301</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>1.058843714293814</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>3.440024914077114</v>
+        <v>1.991721806661441</v>
       </c>
       <c r="L4" t="n">
-        <v>11.46443037825295</v>
+        <v>1.224751774687079</v>
       </c>
       <c r="M4" t="n">
-        <v>10.53313571320021</v>
+        <v>15.9129206383629</v>
       </c>
       <c r="N4" t="n">
-        <v>25.79960979286619</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1247,40 +1247,40 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.03411614863502015</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.05875991450236628</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1108677108962861</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.209184261472802</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.394687099554677</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7788084379023822</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>1.463839042550835</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>3.431536037900564</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>11.15576258712685</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>37.16141177436501</v>
+        <v>37.95991085184107</v>
       </c>
       <c r="M5" t="n">
-        <v>94.64746561101961</v>
+        <v>123.4424162693566</v>
       </c>
       <c r="N5" t="n">
-        <v>34.48099318285622</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1293,40 +1293,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.09854874261732799</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1374080378394981</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2592603264152458</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.4891701963712818</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9229621991398033</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>1.839986032460754</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>3.423137222938942</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>8.023662338646133</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>26.08926650619458</v>
+        <v>9.880521955702118</v>
       </c>
       <c r="L6" t="n">
-        <v>86.89594168379152</v>
+        <v>59.4509121466816</v>
       </c>
       <c r="M6" t="n">
-        <v>171.0792121372329</v>
+        <v>148.3462397177015</v>
       </c>
       <c r="N6" t="n">
-        <v>0.5328430020948771</v>
+        <v>44.74828000197323</v>
       </c>
     </row>
     <row r="7">
@@ -1336,43 +1336,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.004888607537544012</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1535568252959821</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1777716031670491</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3354179609076866</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6328637785515783</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1.198970645120531</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>2.40654073874037</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>4.428682641502151</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>10.37918158852545</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>33.75733421936251</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>112.4125564457501</v>
+        <v>36.40305599183186</v>
       </c>
       <c r="M7" t="n">
-        <v>283.0528681643027</v>
+        <v>282.9786359323118</v>
       </c>
       <c r="N7" t="n">
-        <v>220.154445607015</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1382,43 +1382,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.00505968530910618</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4141801954178035</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5327252756759985</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>1.005141555275961</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1.896492605612812</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>3.583345931923001</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>7.165660493738692</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>13.27136133693284</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>31.1056906218102</v>
+        <v>5.97911736963669</v>
       </c>
       <c r="K8" t="n">
-        <v>101.1520333733247</v>
+        <v>22.91812288184887</v>
       </c>
       <c r="L8" t="n">
-        <v>336.881315850851</v>
+        <v>132.0282440205293</v>
       </c>
       <c r="M8" t="n">
-        <v>553.0560996026129</v>
+        <v>336.2432361675578</v>
       </c>
       <c r="N8" t="n">
-        <v>210.016913114034</v>
+        <v>64.91325517504619</v>
       </c>
     </row>
     <row r="9">
@@ -1434,37 +1434,37 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.009061075949674022</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04952610238075569</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.09344543209552107</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1763120528319958</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0.3326640936504641</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.6367288809960798</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>1.534410664937003</v>
+        <v>0.3529803798301122</v>
       </c>
       <c r="K9" t="n">
-        <v>4.984444617260823</v>
+        <v>1.077469314918521</v>
       </c>
       <c r="L9" t="n">
-        <v>16.60439790710539</v>
+        <v>4.428584755677574</v>
       </c>
       <c r="M9" t="n">
-        <v>53.00296481963424</v>
+        <v>36.1568434829256</v>
       </c>
       <c r="N9" t="n">
-        <v>73.3529984604649</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1498,19 +1498,19 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>3.762510653763389</v>
       </c>
       <c r="K10" t="n">
-        <v>0.06438220879409279</v>
+        <v>8.086290979207718</v>
       </c>
       <c r="L10" t="n">
-        <v>0.2074804937949305</v>
+        <v>11.63060436022849</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>55.80549226999126</v>
       </c>
       <c r="N10" t="n">
-        <v>0.03975999222636958</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1541,22 +1541,22 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>9.831720399319991</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>13.48839262608487</v>
       </c>
       <c r="K11" t="n">
-        <v>0.04092284375570817</v>
+        <v>19.55600740618667</v>
       </c>
       <c r="L11" t="n">
-        <v>0.1318794739876362</v>
+        <v>23.32786577845482</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>141.5531815074712</v>
       </c>
       <c r="N11" t="n">
-        <v>0.02527238471751815</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1572,37 +1572,37 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.001451645253676925</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1213845153127748</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2290272793102955</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4321267381849967</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0.8153330835380983</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>1.53981522790047</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>3.761676132944995</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>12.21956340319206</v>
+        <v>6.882967782317436</v>
       </c>
       <c r="L12" t="n">
-        <v>40.69610472418618</v>
+        <v>15.50416147512446</v>
       </c>
       <c r="M12" t="n">
-        <v>129.9401241477767</v>
+        <v>63.59345048673535</v>
       </c>
       <c r="N12" t="n">
-        <v>24.3059015385701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1612,43 +1612,43 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.0163336607102592</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8241028944310896</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>1.060204620187775</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>2.19048258864527</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>4.249230145297861</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>8.033745245978915</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>15.95128742660574</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>29.60204875987543</v>
+        <v>9.831720399319991</v>
       </c>
       <c r="J13" t="n">
-        <v>69.67733593515047</v>
+        <v>25.44937896450546</v>
       </c>
       <c r="K13" t="n">
-        <v>226.7640770895571</v>
+        <v>102.7883258581555</v>
       </c>
       <c r="L13" t="n">
-        <v>755.1861820410643</v>
+        <v>436.2409331960305</v>
       </c>
       <c r="M13" t="n">
-        <v>1566.835346521528</v>
+        <v>1609.429697790224</v>
       </c>
       <c r="N13" t="n">
-        <v>601.6184781241175</v>
+        <v>404.9460277764708</v>
       </c>
     </row>
   </sheetData>
@@ -1723,43 +1723,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19.06517595244923</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>311.2552537690108</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>280.8592918747708</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>458.7824922166112</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>779.5022243543979</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1318.215992942565</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>2471.333951026047</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>4168.216911052246</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>11453.50744761984</v>
+        <v>2284.748945898546</v>
       </c>
       <c r="K2" t="n">
-        <v>40038.76543247253</v>
+        <v>26929.95822168047</v>
       </c>
       <c r="L2" t="n">
-        <v>131537.0925193689</v>
+        <v>78834.91276201834</v>
       </c>
       <c r="M2" t="n">
-        <v>265412.2091320863</v>
+        <v>290964.8757848679</v>
       </c>
       <c r="N2" t="n">
-        <v>97.1717426960891</v>
+        <v>339546.3562884564</v>
       </c>
     </row>
     <row r="3">
@@ -1778,34 +1778,34 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>73.32184452407334</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>325.4058138175898</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>554.8043246158685</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>979.4017781511488</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>1720.747637724019</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>3850.733114115564</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>12208.17841258754</v>
+        <v>10726.68589256022</v>
       </c>
       <c r="L3" t="n">
-        <v>40120.64940299713</v>
+        <v>52588.65989926519</v>
       </c>
       <c r="M3" t="n">
-        <v>175590.1776582799</v>
+        <v>165188.9657027152</v>
       </c>
       <c r="N3" t="n">
-        <v>17936.72272210229</v>
+        <v>3919.045480274597</v>
       </c>
     </row>
     <row r="4">
@@ -1818,40 +1818,40 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>4.477748101928343</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>42.51807157992635</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>68.42600129504662</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>115.1360501980951</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>190.8800957719636</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>335.4480816854768</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>601.3410942880751</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>1305.15193911284</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>5819.971750632224</v>
+        <v>2545.900473868727</v>
       </c>
       <c r="L4" t="n">
-        <v>16654.64725778939</v>
+        <v>1565.527933227787</v>
       </c>
       <c r="M4" t="n">
-        <v>17021.65264388867</v>
+        <v>19832.03429778211</v>
       </c>
       <c r="N4" t="n">
-        <v>41264.06386169812</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1864,40 +1864,40 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>91.80348552346207</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>137.8472338276812</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>221.8429634721417</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>373.2809472277563</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>618.8496377467558</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>1129.194354114664</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>1949.599390430903</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>4229.779951036992</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>13501.26167107028</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>50373.4987488886</v>
+        <v>48521.91440716817</v>
       </c>
       <c r="M5" t="n">
-        <v>152192.6528157138</v>
+        <v>153844.4317602551</v>
       </c>
       <c r="N5" t="n">
-        <v>53332.95291666834</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1910,40 +1910,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>251.348568045495</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>308.9784620466522</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>504.7150404488798</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>857.5447044506393</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>1439.239564472635</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>2667.004554470889</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>4585.531929732318</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>9937.546516283395</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>41268.56137399755</v>
+        <v>11800.34689378286</v>
       </c>
       <c r="L6" t="n">
-        <v>145472.4959728354</v>
+        <v>71002.46218043042</v>
       </c>
       <c r="M6" t="n">
-        <v>276055.7877367791</v>
+        <v>172741.1854543186</v>
       </c>
       <c r="N6" t="n">
-        <v>618.1138677201203</v>
+        <v>52106.95565517771</v>
       </c>
     </row>
     <row r="7">
@@ -1953,43 +1953,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>16.39140330123432</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>429.378666029131</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>430.01706404887</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>684.7993715279603</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1144.224040259039</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1887.647393971313</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>3490.013510136059</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>5872.654616763927</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>12747.50324339518</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>57210.5797416068</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>188854.0061290132</v>
+        <v>48823.52387485294</v>
       </c>
       <c r="M7" t="n">
-        <v>455298.0935393163</v>
+        <v>370040.6919991546</v>
       </c>
       <c r="N7" t="n">
-        <v>354844.9354293869</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1999,43 +1999,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17.86063854429172</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>1131.262793150509</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>1243.860246175889</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>1948.436750655791</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>3303.121171195834</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>5535.982797146482</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>10370.50214956332</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>17910.76383309782</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>38963.29912978567</v>
+        <v>8653.552652605702</v>
       </c>
       <c r="K8" t="n">
-        <v>170316.7592330028</v>
+        <v>32360.29783667908</v>
       </c>
       <c r="L8" t="n">
-        <v>461501.979952524</v>
+        <v>186423.3524440113</v>
       </c>
       <c r="M8" t="n">
-        <v>688909.3768437783</v>
+        <v>462904.7182589322</v>
       </c>
       <c r="N8" t="n">
-        <v>311817.7787036936</v>
+        <v>89365.81874646537</v>
       </c>
     </row>
     <row r="9">
@@ -2051,37 +2051,37 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>23.68166565903003</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>106.4840916847676</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>174.8177143643008</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>280.6076845642347</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>482.7188863733789</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>834.4968714334622</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>1866.395756402773</v>
+        <v>545.9872276781788</v>
       </c>
       <c r="K9" t="n">
-        <v>6070.704632700475</v>
+        <v>1625.971231717517</v>
       </c>
       <c r="L9" t="n">
-        <v>20330.75688541798</v>
+        <v>6683.022254326578</v>
       </c>
       <c r="M9" t="n">
-        <v>64709.89632939233</v>
+        <v>53198.97393332427</v>
       </c>
       <c r="N9" t="n">
-        <v>83986.2491172939</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -2115,19 +2115,19 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>4363.142804487561</v>
       </c>
       <c r="K10" t="n">
-        <v>108.4846656401343</v>
+        <v>9148.441471908611</v>
       </c>
       <c r="L10" t="n">
-        <v>345.7849161536932</v>
+        <v>13158.30750415322</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>61557.25274727472</v>
       </c>
       <c r="N10" t="n">
-        <v>64.64338576132072</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2158,22 +2158,22 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>12513.5286043629</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>15641.62567134255</v>
       </c>
       <c r="K11" t="n">
-        <v>68.95540095680582</v>
+        <v>22124.7280910041</v>
       </c>
       <c r="L11" t="n">
-        <v>219.7890125530545</v>
+        <v>26392.02760418642</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>156142.7848190832</v>
       </c>
       <c r="N11" t="n">
-        <v>41.08885396912972</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2189,37 +2189,37 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>3.723324911155946</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>257.6932567832552</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>424.8685058485293</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>685.893165184136</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>1182.934157582085</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>2024.025524466052</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>6411.776968604743</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>20780.71171910246</v>
+        <v>10097.98138453456</v>
       </c>
       <c r="L12" t="n">
-        <v>69170.37165583186</v>
+        <v>22746.10878767067</v>
       </c>
       <c r="M12" t="n">
-        <v>208342.0968548207</v>
+        <v>90965.34344523598</v>
       </c>
       <c r="N12" t="n">
-        <v>38945.08064702537</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -2229,43 +2229,43 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>53.31721779797528</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>2219.526514619537</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>2471.485360123976</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>4324.501812608527</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>7497.901171716181</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>12512.12065641595</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>23108.55142310307</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>39667.37780898883</v>
+        <v>12513.5286043629</v>
       </c>
       <c r="J13" t="n">
-        <v>90765.694066357</v>
+        <v>31489.05730201254</v>
       </c>
       <c r="K13" t="n">
-        <v>367392.9340337696</v>
+        <v>127360.3114977362</v>
       </c>
       <c r="L13" t="n">
-        <v>1124581.072453373</v>
+        <v>556739.8196513109</v>
       </c>
       <c r="M13" t="n">
-        <v>2303531.943554055</v>
+        <v>1997381.258202944</v>
       </c>
       <c r="N13" t="n">
-        <v>902948.8012480151</v>
+        <v>484938.1761703741</v>
       </c>
     </row>
   </sheetData>
@@ -2340,43 +2340,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.02915693088405939</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5864033008213906</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1.156736447362879</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>2.232836216071437</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>4.263212180078946</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8.094108417671119</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>15.32221111557303</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>28.96013429885784</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>93.45935233249475</v>
+        <v>17.04003054828831</v>
       </c>
       <c r="K2" t="n">
-        <v>301.3169244422875</v>
+        <v>222.9093222562142</v>
       </c>
       <c r="L2" t="n">
-        <v>971.166445111608</v>
+        <v>817.0522416429498</v>
       </c>
       <c r="M2" t="n">
-        <v>2324.628290376588</v>
+        <v>2986.947953066119</v>
       </c>
       <c r="N2" t="n">
-        <v>1856.45768584063</v>
+        <v>5244.942033066807</v>
       </c>
     </row>
     <row r="3">
@@ -2395,34 +2395,34 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1781833457686076</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1.045182193931899</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>2.681028305343615</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>5.767528945903679</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>11.59111231216325</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>39.20476700994847</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>128.1935547432587</v>
+        <v>89.89910095895924</v>
       </c>
       <c r="L3" t="n">
-        <v>414.9721224088885</v>
+        <v>530.6385141321756</v>
       </c>
       <c r="M3" t="n">
-        <v>1339.15537028974</v>
+        <v>1905.615769533023</v>
       </c>
       <c r="N3" t="n">
-        <v>1255.857830410614</v>
+        <v>1673.983736714836</v>
       </c>
     </row>
     <row r="4">
@@ -2435,40 +2435,40 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.007598298852421526</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.09035678609865967</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2465048015601257</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5411235596339394</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1.09700774652184</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>2.145845340069105</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>4.124783262006889</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>13.49113147749768</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>43.67547260534667</v>
+        <v>18.18442009481895</v>
       </c>
       <c r="L4" t="n">
-        <v>140.948649766913</v>
+        <v>29.36640379771198</v>
       </c>
       <c r="M4" t="n">
-        <v>216.5988908538056</v>
+        <v>165.5591591785558</v>
       </c>
       <c r="N4" t="n">
-        <v>384.1548921935422</v>
+        <v>150.8759572796998</v>
       </c>
     </row>
     <row r="5">
@@ -2481,40 +2481,40 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1557815006165304</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4240916124994815</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9303368677336648</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1.885516143865181</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>3.687740342744984</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>7.08816175492472</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>13.50404818436978</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>43.85844194769599</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>141.6796370390724</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>456.9218482232159</v>
+        <v>346.5739860773089</v>
       </c>
       <c r="M5" t="n">
-        <v>1254.673595241534</v>
+        <v>1473.603246616534</v>
       </c>
       <c r="N5" t="n">
-        <v>1348.942143206012</v>
+        <v>1300.31625357788</v>
       </c>
     </row>
     <row r="6">
@@ -2527,40 +2527,40 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4499942585266118</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1.077428221264046</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>2.261265328182977</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>4.494919192892025</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>8.709358458370579</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>16.66112690514422</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>31.66445651747043</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>102.6392476256503</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>331.36524168425</v>
+        <v>90.20916545556032</v>
       </c>
       <c r="L6" t="n">
-        <v>1068.466112870403</v>
+        <v>632.9959933547632</v>
       </c>
       <c r="M6" t="n">
-        <v>2475.066548622116</v>
+        <v>1942.292579249597</v>
       </c>
       <c r="N6" t="n">
-        <v>1964.01850211163</v>
+        <v>2034.346378990231</v>
       </c>
     </row>
     <row r="7">
@@ -2570,43 +2570,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.02232240884723293</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7234951270937264</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1.535237607308562</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>3.066826469900738</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>5.956615413058629</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>11.40904480841473</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>21.69664258669961</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>41.10719527316126</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>132.9177584095422</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>428.7898841399463</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1382.278369492012</v>
+        <v>332.3599012054248</v>
       </c>
       <c r="M7" t="n">
-        <v>3765.699467760128</v>
+        <v>2915.954847267431</v>
       </c>
       <c r="N7" t="n">
-        <v>5108.799926887605</v>
+        <v>2749.774896664719</v>
       </c>
     </row>
     <row r="8">
@@ -2616,43 +2616,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.02310358588632959</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>1.914337354917396</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>4.346872860287252</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>8.936560327300771</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>17.59634391457388</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>33.93555052011678</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>64.76422768139936</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>122.9315156323438</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>398.082170360828</v>
+        <v>54.58934158478297</v>
       </c>
       <c r="K8" t="n">
-        <v>1284.792874767451</v>
+        <v>263.8318034960631</v>
       </c>
       <c r="L8" t="n">
-        <v>4142.339676119458</v>
+        <v>1441.955000611104</v>
       </c>
       <c r="M8" t="n">
-        <v>8589.163763836768</v>
+        <v>4379.939845072875</v>
       </c>
       <c r="N8" t="n">
-        <v>8506.974161114817</v>
+        <v>4265.26769991169</v>
       </c>
     </row>
     <row r="9">
@@ -2668,37 +2668,37 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0.04137477602590878</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2675213622394051</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.694212832995209</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>1.499290699807975</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>3.018304826065802</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>5.88436786280738</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>19.4577583260288</v>
+        <v>3.222710867848924</v>
       </c>
       <c r="K9" t="n">
-        <v>63.19986982747471</v>
+        <v>13.06000571305502</v>
       </c>
       <c r="L9" t="n">
-        <v>204.1648206103627</v>
+        <v>51.8816290984668</v>
       </c>
       <c r="M9" t="n">
-        <v>658.4436989531511</v>
+        <v>375.4636072410501</v>
       </c>
       <c r="N9" t="n">
-        <v>1229.754906243396</v>
+        <v>350.3284704087789</v>
       </c>
     </row>
     <row r="10">
@@ -2732,19 +2732,19 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>0</v>
+        <v>34.35172226885974</v>
       </c>
       <c r="K10" t="n">
-        <v>0.5879653771150026</v>
+        <v>108.1795589090262</v>
       </c>
       <c r="L10" t="n">
-        <v>2.482764407205692</v>
+        <v>197.1911155834824</v>
       </c>
       <c r="M10" t="n">
-        <v>2.188781718648191</v>
+        <v>652.6054805539895</v>
       </c>
       <c r="N10" t="n">
-        <v>1.310504466884336</v>
+        <v>562.5978533294632</v>
       </c>
     </row>
     <row r="11">
@@ -2775,22 +2775,22 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>44.88180362289576</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>168.0308282990506</v>
       </c>
       <c r="K11" t="n">
-        <v>0.3737246005087504</v>
+        <v>346.5771759175348</v>
       </c>
       <c r="L11" t="n">
-        <v>1.578103358386706</v>
+        <v>453.1042745138542</v>
       </c>
       <c r="M11" t="n">
-        <v>1.391241058132331</v>
+        <v>1594.637135529747</v>
       </c>
       <c r="N11" t="n">
-        <v>0.8329874128889153</v>
+        <v>1398.872254441858</v>
       </c>
     </row>
     <row r="12">
@@ -2806,37 +2806,37 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.006628517140077284</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5608957103490945</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>1.606682373866426</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>3.579863826765953</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>7.302845943378275</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>14.3273371883408</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>47.60338335693471</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>154.8400038444915</v>
+        <v>62.84149585255818</v>
       </c>
       <c r="L12" t="n">
-        <v>500.4247140990935</v>
+        <v>204.3944901204445</v>
       </c>
       <c r="M12" t="n">
-        <v>1614.118818023369</v>
+        <v>753.581945138059</v>
       </c>
       <c r="N12" t="n">
-        <v>1594.466466195798</v>
+        <v>651.3847000778368</v>
       </c>
     </row>
     <row r="13">
@@ -2846,43 +2846,43 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.07458292561762192</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>3.837609840828077</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>8.678726827986868</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>18.68093042910682</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>38.08380780489613</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>74.69299312575758</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>143.7668950991578</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>274.0949505315215</v>
+        <v>44.88180362289576</v>
       </c>
       <c r="J13" t="n">
-        <v>890.7140108466208</v>
+        <v>277.2346335688305</v>
       </c>
       <c r="K13" t="n">
-        <v>2878.815153071203</v>
+        <v>1215.69204865379</v>
       </c>
       <c r="L13" t="n">
-        <v>9285.743626467547</v>
+        <v>5037.513550137685</v>
       </c>
       <c r="M13" t="n">
-        <v>22241.12846673398</v>
+        <v>19146.20156844698</v>
       </c>
       <c r="N13" t="n">
-        <v>23251.57000608382</v>
+        <v>20382.6902344638</v>
       </c>
     </row>
   </sheetData>

</xml_diff>